<commit_message>
Update to identify incentive_PROJECT_models.qmd as core file.
</commit_message>
<xml_diff>
--- a/ptax_file_inventory.xlsx
+++ b/ptax_file_inventory.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mvh/Library/CloudStorage/GoogleDrive-michael.vanhulle@gmail.com/My Drive/PhD/Cook County Property Taxes/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micha\Data Analysis\ptax\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52ADA067-8E7A-C146-B66F-4C32496CCE91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8E79A00-F0B8-4583-AF59-4C6474D8AAB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="1820" windowWidth="34520" windowHeight="17440" activeTab="1" xr2:uid="{8104F543-8E88-1346-A6A2-DCE31E170ED6}"/>
+    <workbookView xWindow="59310" yWindow="6915" windowWidth="28800" windowHeight="15375" activeTab="1" xr2:uid="{8104F543-8E88-1346-A6A2-DCE31E170ED6}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="3" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="132">
   <si>
     <t>File</t>
   </si>
@@ -84,9 +84,6 @@
     <t>incentive_PROJECT_models.qmd</t>
   </si>
   <si>
-    <t>Joins multiple inputs: project-level crosswalks, BOR appeals, proration data</t>
-  </si>
-  <si>
     <t>seniorfreeze.qmd</t>
   </si>
   <si>
@@ -372,18 +369,9 @@
     <t>Likely reads muni_shortnames.xlsx</t>
   </si>
   <si>
-    <t>incentivePINs_allyears.csv, PIN-level datasets</t>
-  </si>
-  <si>
     <t>ptax_pull_loop_* scripts</t>
   </si>
   <si>
-    <t>Pulls from comm_ind_PINs_2011-2022_balanced.csv</t>
-  </si>
-  <si>
-    <t>Pulls from comm_ind_PINs_2006to2022_timeseries.csv</t>
-  </si>
-  <si>
     <t>Pulls from ptaxsim.db and queries for freeze exemptions</t>
   </si>
   <si>
@@ -399,12 +387,6 @@
     <t>Outputs</t>
   </si>
   <si>
-    <t>./Output/incentivePINs_allyears.csv, ./Necessary_Files/Assessor_-_Commercial_Valuation_Data_20240212.csv, ./Necessary_Files/Assessor_-_Commercial_Valuation_Data_20240301.csv, incentivePINs_accessDB_2.xlsx</t>
-  </si>
-  <si>
-    <t>./Output/comm_ind_PINs_2011-2022_balanced.csv, ./Output/comm_ind_PINs_2006to2022_timeseries.csv</t>
-  </si>
-  <si>
     <t>Summary of PTAX GitHub Files, Inputs, and Outputs</t>
   </si>
   <si>
@@ -430,13 +412,76 @@
   </si>
   <si>
     <t>Output/</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>./Output/incentivePINs_allyears.csv,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ./Necessary_Files/Assessor_-_Commercial_Valuation_Data_20240212.csv, ./Necessary_Files/Assessor_-_Commercial_Valuation_Data_20240301.csv, incentivePINs_accessDB_2.xlsx</t>
+    </r>
+  </si>
+  <si>
+    <t>I don't think we need this file?</t>
+  </si>
+  <si>
+    <t>Makes an old verison of the pin-project crosswalk; likely deprecated by incentive_Project_models.qmd</t>
+  </si>
+  <si>
+    <t>I think we want to pull the part of this document that makes the project data and put it in a separate script; jw did you do pre-2011 in a fit of nerd rage?</t>
+  </si>
+  <si>
+    <t>comm_ind_2011-2022 timeseries.csv</t>
+  </si>
+  <si>
+    <t>Causal models using incentive class change as exogenous shock; does not aggregate to project level.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">This is the important document. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Creates pin-project crosswalk w/ models and pictures with lots of inputs.</t>
+    </r>
+  </si>
+  <si>
+    <t>Beautiful models presented beautifully for the white paper.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -458,8 +503,31 @@
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -469,6 +537,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -485,7 +571,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -498,6 +584,27 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -840,24 +947,24 @@
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="33.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -870,10 +977,10 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="56.6640625" style="3" customWidth="1"/>
     <col min="2" max="2" width="62.33203125" style="3" customWidth="1"/>
@@ -884,27 +991,27 @@
     <col min="7" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -912,7 +1019,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="32" x14ac:dyDescent="0.4">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
@@ -920,57 +1027,61 @@
         <v>4</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="85" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="64" x14ac:dyDescent="0.4">
+      <c r="A4" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="80" x14ac:dyDescent="0.4">
+      <c r="A6" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="C6" s="7"/>
+      <c r="D6" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A7" s="3" t="s">
         <v>109</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="85" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>111</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
@@ -978,66 +1089,66 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A9" s="11" t="s">
         <v>11</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="32" x14ac:dyDescent="0.4">
+      <c r="A10" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="48" x14ac:dyDescent="0.4">
+      <c r="A11" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A12" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A13" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A14" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="E9" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="51" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="B14" s="3" t="s">
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A15" s="3" t="s">
         <v>116</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
-        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -1053,272 +1164,272 @@
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="57.1640625" customWidth="1"/>
     <col min="3" max="3" width="50.1640625" customWidth="1"/>
     <col min="4" max="4" width="32.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A2" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="B2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>94</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A3" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>95</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>96</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>98</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A5" s="1" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>100</v>
-      </c>
       <c r="B5" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>100</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>101</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A7" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>95</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>96</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A9" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>95</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>96</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="1" t="s">
+      <c r="D11" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="D10" s="1" t="s">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A12" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>104</v>
-      </c>
       <c r="B12" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A13" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A14" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>106</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>107</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A16" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A17" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -1334,329 +1445,329 @@
       <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="46.6640625" customWidth="1"/>
     <col min="2" max="2" width="42.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
         <v>26</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A7" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A8" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A9" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A10" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="B10" t="s">
         <v>36</v>
       </c>
-      <c r="B10" t="s">
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A11" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A12" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A13" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A14" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A15" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A16" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A17" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A18" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A19" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A20" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A21" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A22" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A23" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A24" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A25" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A26" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A27" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A28" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A29" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A30" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A31" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A32" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A33" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A34" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A35" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A36" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
+      <c r="B36" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A37" t="s">
         <v>63</v>
       </c>
-      <c r="B36" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A38" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A39" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A40" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A41" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A42" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A43" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A44" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A45" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A46" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A47" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A48" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A49" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A50" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A51" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A52" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A53" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A54" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A55" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A56" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A57" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A58" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A59" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A60" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A61" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A62" t="s">
         <v>88</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
-        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -1672,7 +1783,7 @@
       <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added file names, inputs, outputs, etc. to file inventory
</commit_message>
<xml_diff>
--- a/ptax_file_inventory.xlsx
+++ b/ptax_file_inventory.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micha\Data Analysis\ptax\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleaw\Documents\PhD Fall 2021 - Spring 2022\Merriman RA\ptax\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8E79A00-F0B8-4583-AF59-4C6474D8AAB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DF53163-6D17-482C-A2B6-23DED00F53E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="59310" yWindow="6915" windowWidth="28800" windowHeight="15375" activeTab="1" xr2:uid="{8104F543-8E88-1346-A6A2-DCE31E170ED6}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12360" activeTab="1" xr2:uid="{8104F543-8E88-1346-A6A2-DCE31E170ED6}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="3" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Changes to files" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="160">
   <si>
     <t>File</t>
   </si>
@@ -48,15 +49,9 @@
     <t>combine_CCAOmethodology_sheets.R</t>
   </si>
   <si>
-    <t>Reads CCAO spreadsheet files</t>
-  </si>
-  <si>
     <t>helper_clean_commercial_valuation_properties.R</t>
   </si>
   <si>
-    <t>Reads commercial valuation CSVs</t>
-  </si>
-  <si>
     <t>helper_pull_comm_ind_allyears.R</t>
   </si>
   <si>
@@ -72,9 +67,6 @@
     <t>0_joined_PIN_level_data_allyears.qmd</t>
   </si>
   <si>
-    <t>Merges all parcel-level annual data into master</t>
-  </si>
-  <si>
     <t>incentive_models_OLS.qmd</t>
   </si>
   <si>
@@ -366,9 +358,6 @@
     <t>incentivePINs_accessDB_2.xlsx</t>
   </si>
   <si>
-    <t>Likely reads muni_shortnames.xlsx</t>
-  </si>
-  <si>
     <t>ptax_pull_loop_* scripts</t>
   </si>
   <si>
@@ -403,9 +392,6 @@
   </si>
   <si>
     <t>Moved creation of time series data to new file, helper_comm_ind_timeseries.R; frontloaded loading of necessary files, creation of function, scipen</t>
-  </si>
-  <si>
-    <t>- What if we update the cde/nicknames/loa necessary files so we don't need to clean them up each time we use them? - What if we go back and excise the Aleacat entirely? Replace it with an ocelot? (Jk but maybe we can find a way to remove it) - ~line 115, do we need "AND year &lt;= 2023"?</t>
   </si>
   <si>
     <t>Pulls all PINs that were EVER comm/ind from 2006-2023 that are within municipalities (i.e., no unincorporated areas of the county) for all years.</t>
@@ -445,10 +431,79 @@
     <t>I think we want to pull the part of this document that makes the project data and put it in a separate script; jw did you do pre-2011 in a fit of nerd rage?</t>
   </si>
   <si>
-    <t>comm_ind_2011-2022 timeseries.csv</t>
-  </si>
-  <si>
     <t>Causal models using incentive class change as exogenous shock; does not aggregate to project level.</t>
+  </si>
+  <si>
+    <t>Beautiful models presented beautifully for the white paper.</t>
+  </si>
+  <si>
+    <t>commercial_sales_data.qmd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">archive? </t>
+  </si>
+  <si>
+    <t>./Inputs/parceluniverse_keypins_20240725.xlsx</t>
+  </si>
+  <si>
+    <t>Uses sales data to creat project identifier. First one that did this? See if it is incorporated into anotehr file.</t>
+  </si>
+  <si>
+    <t>Which file creates ./Inputs/parceluniverse_keypins_20240725.xlsx????</t>
+  </si>
+  <si>
+    <t>Files</t>
+  </si>
+  <si>
+    <t>Made by</t>
+  </si>
+  <si>
+    <t>- What if we update the cde/nicknames/loa necessary files so we don't need to clean them up each time we use them? - What if we go back and excise the Aleacat entirely? (Jk but maybe we can find a way to remove it) - ~line 115, do we need "AND year &lt;= 2023"?</t>
+  </si>
+  <si>
+    <t>Produces list of tax codes and the municipality they are in.</t>
+  </si>
+  <si>
+    <t>all_keypins_2022.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">parceluniverse_keypins_20240725.xlsx, Assessor_-_Commercial_Valuation_Data_20240301.csv, amazonPINs.xlsx, helper_tc_muninames_2022.R, ptaxsim database, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uses an archived parcel universe, ptaxsim, and the more current parcel universe to create keypins. </t>
+  </si>
+  <si>
+    <t>Might be old and redundant for a newer/better version in other files.</t>
+  </si>
+  <si>
+    <t>methodology_reports/north_2022 folder, south_2023 folder,</t>
+  </si>
+  <si>
+    <t>Output/combined_methodologyworksheets_NORTH.csv, Output/combined_methodologyworksheets_SOUTH.csv, Output/combined_methodologyworksheets_CHICAGO.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Combines the methodology worksheets found online and attempts to combine them. These worksheets become the "Commercial Valuation dataset" posted by the Assessor after significant data cleaning. This R script was an attempt to create them from scratch and see if it could be done better. Then got distracted with making keypins from the sales and appeals data identifiers. </t>
+  </si>
+  <si>
+    <t>Last ran and created files in May 2024, so the files are probably not used. It is a good example of how to read in a bunch of excel files though!</t>
+  </si>
+  <si>
+    <t>Reads CCAO methodology spreadsheet files and combines them into 3 larget files for the Chicago, north, south, and triads for 2021, 2022, and 2023.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">comm_ind_2011-2022 timeseries.csv, parceluniverse_keypins_20240724.xlsx, borappeals.csv, all_keypins.csv, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">all commented out or set to eval=FALSE: (incentive_project_summaries.csv, project_summaries.csv,  block_panel_summaries.csv, properties_were_exempt.csv, properties_became_exempt.csv, project_panel_summaries.csv), </t>
+  </si>
+  <si>
+    <t>UNFINISHED and was abandoned. Was an attempt at using project level data for models. Needs good project level input to run the models.</t>
+  </si>
+  <si>
+    <t>muni_ratechange_YEAR.csv, muni_mc_burden_YEAR.csv,  muni_burden_shift_YEAR.csv, 0_joined_PIN_data_YEAR.csv</t>
+  </si>
+  <si>
+    <t>muni_shortnames.xlsx, ptaxsim database, eq_factor.csv, ccao_loa.csv</t>
   </si>
   <si>
     <r>
@@ -460,7 +515,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">This is the important document. </t>
+      <t>CRITICAL FILE for website.</t>
     </r>
     <r>
       <rPr>
@@ -470,11 +525,53 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Creates pin-project crosswalk w/ models and pictures with lots of inputs.</t>
+      <t xml:space="preserve"> Creates files for each year used to render website faster. </t>
     </r>
   </si>
   <si>
-    <t>Beautiful models presented beautifully for the white paper.</t>
+    <t>None</t>
+  </si>
+  <si>
+    <t>incentive_commerc_indust_breakdown</t>
+  </si>
+  <si>
+    <t>combine_commercial_projects.qmd</t>
+  </si>
+  <si>
+    <t>0_joined_PIN_data_2022.csv, class_dict_expanded.csv, parceluniverse_keypins_20240725.xlsx</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">This is the important file for creating project identifiers! </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Tables with project identifiers that have number pins with and without incentive classification, summed AV and summed FMV</t>
+    </r>
+  </si>
+  <si>
+    <t>mapping_com_ind_projects</t>
+  </si>
+  <si>
+    <t>Identifies parcels that are owned by the same person. Maps a couple municipalities with the pins grouped by color</t>
+  </si>
+  <si>
+    <t>maps of parcels color coded by project identifier or owner or proximity. Different ways to visualize PINs that are potentially part of the same project</t>
+  </si>
+  <si>
+    <t>Building block for what became the website and most of the incentive report. Can be archived once sure that everything we want from it is part of another file or the website.</t>
+  </si>
+  <si>
+    <t>incentive_report_appendices.qmd</t>
+  </si>
+  <si>
+    <t>Needs to be added to  website still I think! Makes amazon images? Maybe?</t>
   </si>
 </sst>
 </file>
@@ -571,7 +668,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -607,11 +704,54 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="8">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -622,6 +762,38 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{54438E1D-7E74-4957-AE8D-E2C5ABC9DAFB}" name="Table1" displayName="Table1" ref="A1:F21" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+  <autoFilter ref="A1:F21" xr:uid="{54438E1D-7E74-4957-AE8D-E2C5ABC9DAFB}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F20">
+    <sortCondition ref="A1:A20"/>
+  </sortState>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{457F3B97-D78E-4D53-8E6B-FE920F1B7B60}" name="File" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{6B0D2B68-1EEC-48E8-BFB0-5D91728A5149}" name="Description" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{1BF32799-F320-46B3-A0F1-B24BE715E5B8}" name="Changes" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{FD59E246-87F8-4AEC-87F7-84E2B50D8F33}" name="Thoughts" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{7CFEA2D0-A2F5-4DC1-A26D-C81D47F75D97}" name="Inputs" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{F74E7965-C3AC-4B04-BEEC-DB75BB8668F0}" name="Outputs" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D84FAE05-F6C9-4A54-9026-E207569C7562}" name="Table2" displayName="Table2" ref="A1:B63" totalsRowShown="0">
+  <autoFilter ref="A1:B63" xr:uid="{D84FAE05-F6C9-4A54-9026-E207569C7562}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B63">
+    <sortCondition ref="A1:A63"/>
+  </sortState>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{D5BACC63-C394-43D2-B577-97F67FEFF3A5}" name="Files"/>
+    <tableColumn id="2" xr3:uid="{5E632370-997E-4620-ADF6-1E674D713A67}" name="Made by"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -947,24 +1119,24 @@
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="10.6484375" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
   <cols>
     <col min="1" max="1" width="33.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.6">
       <c r="A1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.4">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.6">
       <c r="A2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.6">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -974,462 +1146,558 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44549863-5D02-D84A-9B87-3FF43E548FC8}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="74" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="10.84765625" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
   <cols>
-    <col min="1" max="1" width="56.6640625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="62.33203125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="50.6640625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="58.83203125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="61.33203125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="44.33203125" style="3" customWidth="1"/>
-    <col min="7" max="16384" width="10.83203125" style="3"/>
+    <col min="1" max="1" width="36.09765625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="40.69921875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="31.25" style="3" customWidth="1"/>
+    <col min="4" max="4" width="28.84765625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="37.1484375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="26.34765625" style="3" customWidth="1"/>
+    <col min="7" max="16384" width="10.84765625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.6">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="62.4" x14ac:dyDescent="0.6">
+      <c r="A2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="46.8" x14ac:dyDescent="0.6">
+      <c r="A3" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="171.6" x14ac:dyDescent="0.6">
+      <c r="A4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="62.4" x14ac:dyDescent="0.6">
+      <c r="A5" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="46.8" x14ac:dyDescent="0.6">
+      <c r="A6" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="93.6" x14ac:dyDescent="0.6">
+      <c r="A7" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="124.8" x14ac:dyDescent="0.6">
+      <c r="A8" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="F8" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="32" x14ac:dyDescent="0.4">
-      <c r="A3" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="3" t="s">
+    </row>
+    <row r="9" spans="1:6" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="A9" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="B9" s="3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="62.4" x14ac:dyDescent="0.6">
+      <c r="A10" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="A11" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="140.4" x14ac:dyDescent="0.6">
+      <c r="A12" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="93.6" x14ac:dyDescent="0.6">
+      <c r="A13" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="93.6" x14ac:dyDescent="0.6">
+      <c r="A14" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="C14" s="7"/>
+      <c r="D14" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="A15" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.6">
+      <c r="A16" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A17" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="A18" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="64" x14ac:dyDescent="0.4">
-      <c r="A4" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="80" x14ac:dyDescent="0.4">
-      <c r="A6" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>126</v>
-      </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A7" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A9" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="32" x14ac:dyDescent="0.4">
-      <c r="A10" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="3" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A19" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="46.8" x14ac:dyDescent="0.6">
+      <c r="B20" s="3" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="48" x14ac:dyDescent="0.4">
-      <c r="A11" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A12" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A13" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A14" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A15" s="3" t="s">
-        <v>116</v>
+    <row r="21" spans="1:2" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="A21" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>159</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB19EFBB-84B3-DC40-9462-4782F856E273}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="10.6484375" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
   <cols>
-    <col min="1" max="1" width="57.1640625" customWidth="1"/>
-    <col min="3" max="3" width="50.1640625" customWidth="1"/>
-    <col min="4" max="4" width="32.1640625" customWidth="1"/>
+    <col min="1" max="1" width="57.1484375" customWidth="1"/>
+    <col min="3" max="3" width="50.1484375" customWidth="1"/>
+    <col min="4" max="4" width="32.1484375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.6">
+      <c r="A2" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A2" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>93</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A3" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>95</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.6">
+      <c r="A4" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>94</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A4" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>97</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A5" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A6" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A7" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A8" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A9" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A10" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A11" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A12" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.6">
+      <c r="A13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>94</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A13" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>97</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A14" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A15" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A16" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A17" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.6">
+      <c r="A18" t="s">
+        <v>127</v>
+      </c>
+      <c r="C18" t="s">
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -1439,339 +1707,350 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B518CB6C-64CD-4548-9867-37ED0B4CBCF0}">
-  <dimension ref="A1:B62"/>
+  <dimension ref="A1:B63"/>
   <sheetViews>
-    <sheetView topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="B55" sqref="B55"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="10.6484375" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
   <cols>
-    <col min="1" max="1" width="46.6640625" customWidth="1"/>
+    <col min="1" max="1" width="46.6484375" customWidth="1"/>
     <col min="2" max="2" width="42.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A7" t="s">
         <v>25</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A9" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A10" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A11" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A12" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A15" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.6">
+      <c r="A17" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.6">
+      <c r="A18" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.6">
+      <c r="A19" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.6">
+      <c r="A20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.6">
+      <c r="A21" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.6">
+      <c r="A22" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.6">
+      <c r="A23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.6">
+      <c r="A24" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.6">
+      <c r="A25" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.6">
+      <c r="A26" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.6">
+      <c r="A27" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.6">
+      <c r="A28" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.6">
+      <c r="A29" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.6">
+      <c r="A30" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.6">
+      <c r="A31" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.6">
+      <c r="A32" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A33" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A34" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A35" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A36" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A5" t="s">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A37" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A7" t="s">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A38" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A39" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A40" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A41" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A42" t="s">
+        <v>22</v>
+      </c>
+      <c r="B42" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A43" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A44" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A45" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A46" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A47" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A48" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A8" t="s">
+      <c r="B48" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A10" t="s">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.6">
+      <c r="A49" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.6">
+      <c r="A50" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.6">
+      <c r="A51" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.6">
+      <c r="A52" t="s">
         <v>35</v>
       </c>
-      <c r="B10" t="s">
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.6">
+      <c r="A53" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.6">
+      <c r="A54" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A12" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A13" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A14" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A15" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A16" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A17" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A18" t="s">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.6">
+      <c r="A55" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.6">
+      <c r="A56" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.6">
+      <c r="A57" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.6">
+      <c r="A58" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.6">
+      <c r="A59" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.6">
+      <c r="A60" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.6">
+      <c r="A61" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.6">
+      <c r="A62" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A19" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A20" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A21" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A22" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A23" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A24" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A25" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A26" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A27" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A28" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A29" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A30" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A31" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A32" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A33" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A34" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A35" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A36" t="s">
-        <v>62</v>
-      </c>
-      <c r="B36" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A37" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A38" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A39" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A40" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A41" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A42" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A43" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A44" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A45" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A46" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A47" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A48" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A49" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A50" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A51" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A52" t="s">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.6">
+      <c r="A63" t="s">
         <v>78</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A53" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A54" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A55" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A56" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A57" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A58" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A59" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A60" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A61" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A62" t="s">
-        <v>88</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -1783,7 +2062,7 @@
       <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="10.6484375" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added inputs and outputs to files
</commit_message>
<xml_diff>
--- a/ptax_file_inventory.xlsx
+++ b/ptax_file_inventory.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleaw\Documents\PhD Fall 2021 - Spring 2022\Merriman RA\ptax\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DF53163-6D17-482C-A2B6-23DED00F53E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80B686D0-42AA-4E4E-9CA2-3490E9DFB11C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12360" activeTab="1" xr2:uid="{8104F543-8E88-1346-A6A2-DCE31E170ED6}"/>
+    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" activeTab="1" xr2:uid="{8104F543-8E88-1346-A6A2-DCE31E170ED6}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="3" r:id="rId1"/>
@@ -20,7 +20,6 @@
     <sheet name="Changes to files" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -41,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="172">
   <si>
     <t>File</t>
   </si>
@@ -364,9 +363,6 @@
     <t>Pulls from ptaxsim.db and queries for freeze exemptions</t>
   </si>
   <si>
-    <t>propFMV_sankey.qmd, agency_revenue_graphs.qmd, etc.</t>
-  </si>
-  <si>
     <t>Typically build visualizations based on ptaxsim or merged PIN-level datasets</t>
   </si>
   <si>
@@ -395,9 +391,6 @@
   </si>
   <si>
     <t>Pulls all PINs that were EVER comm/ind from 2006-2023 that are within municipalities (i.e., no unincorporated areas of the county) for all years.</t>
-  </si>
-  <si>
-    <t>Output/</t>
   </si>
   <si>
     <r>
@@ -425,9 +418,6 @@
     <t>I don't think we need this file?</t>
   </si>
   <si>
-    <t>Makes an old verison of the pin-project crosswalk; likely deprecated by incentive_Project_models.qmd</t>
-  </si>
-  <si>
     <t>I think we want to pull the part of this document that makes the project data and put it in a separate script; jw did you do pre-2011 in a fit of nerd rage?</t>
   </si>
   <si>
@@ -438,9 +428,6 @@
   </si>
   <si>
     <t>commercial_sales_data.qmd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">archive? </t>
   </si>
   <si>
     <t>./Inputs/parceluniverse_keypins_20240725.xlsx</t>
@@ -572,6 +559,54 @@
   </si>
   <si>
     <t>Needs to be added to  website still I think! Makes amazon images? Maybe?</t>
+  </si>
+  <si>
+    <t>Joined Commercial valuation data to CMAP's Access database for incentive projects in order to try to make a project identifier. Makes an old verison of the pin-project crosswalk; likely deprecated by combine_com_ind_projects.qmd</t>
+  </si>
+  <si>
+    <t>manually_cleaned_incentive_pins_AWM.csv, project_pins_wide.csv, project_MC_pins_wide.csv, incentive_crosswalk.csv</t>
+  </si>
+  <si>
+    <t>html output with summary tables of projects that had at least 1 incentive pin in them.</t>
+  </si>
+  <si>
+    <t>Moved to old_files folder</t>
+  </si>
+  <si>
+    <t>properties_were_exempt.csv, properties_became_exempt.csv, project_panel_summaries.csv</t>
+  </si>
+  <si>
+    <t>sales data, parceluniverse_keypins_20240725,  board of review appeals data, all_keypins.csv</t>
+  </si>
+  <si>
+    <t>Output/comm_ind_PINs_ever_2006to2023.csv</t>
+  </si>
+  <si>
+    <t>helper_comm_ind_timeseries.R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Creates timeseries of all pins that were commercial or industrial type between 2006 and 2023. </t>
+  </si>
+  <si>
+    <t>Originally was part of helper_pull_com_ind_allyears.R</t>
+  </si>
+  <si>
+    <t>comm_ind_pins_ever, Triad_reassessment_years.csv</t>
+  </si>
+  <si>
+    <t>comm_ind_PINs_2006to2023_timeseries.csv, comm_ind_PINs_2011to2023_timeseries.csv, dropped_frompanel_2006to2022.csv, comm_ind_PINs_2006to2022_balanced.csv, pin_class_changes.csv, comm_ind_PINs_2011-2022_balanced.csv,</t>
+  </si>
+  <si>
+    <t>Still torn about using balanced or timeseries versions of data in models.</t>
+  </si>
+  <si>
+    <t>propFMV_sankey.qmd</t>
+  </si>
+  <si>
+    <t>agency_revenue_graphs.qmd</t>
+  </si>
+  <si>
+    <t>Recreates all models included in the incentive report</t>
   </si>
 </sst>
 </file>
@@ -668,7 +703,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -707,27 +742,15 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="8">
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </font>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -749,6 +772,21 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
@@ -765,18 +803,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{54438E1D-7E74-4957-AE8D-E2C5ABC9DAFB}" name="Table1" displayName="Table1" ref="A1:F21" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
-  <autoFilter ref="A1:F21" xr:uid="{54438E1D-7E74-4957-AE8D-E2C5ABC9DAFB}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{54438E1D-7E74-4957-AE8D-E2C5ABC9DAFB}" name="Table1" displayName="Table1" ref="A1:F23" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:F23" xr:uid="{54438E1D-7E74-4957-AE8D-E2C5ABC9DAFB}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F20">
     <sortCondition ref="A1:A20"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{457F3B97-D78E-4D53-8E6B-FE920F1B7B60}" name="File" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{6B0D2B68-1EEC-48E8-BFB0-5D91728A5149}" name="Description" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{1BF32799-F320-46B3-A0F1-B24BE715E5B8}" name="Changes" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{FD59E246-87F8-4AEC-87F7-84E2B50D8F33}" name="Thoughts" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{7CFEA2D0-A2F5-4DC1-A26D-C81D47F75D97}" name="Inputs" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{F74E7965-C3AC-4B04-BEEC-DB75BB8668F0}" name="Outputs" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{457F3B97-D78E-4D53-8E6B-FE920F1B7B60}" name="File" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{6B0D2B68-1EEC-48E8-BFB0-5D91728A5149}" name="Description" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{1BF32799-F320-46B3-A0F1-B24BE715E5B8}" name="Changes" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{FD59E246-87F8-4AEC-87F7-84E2B50D8F33}" name="Thoughts" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{7CFEA2D0-A2F5-4DC1-A26D-C81D47F75D97}" name="Inputs" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{F74E7965-C3AC-4B04-BEEC-DB75BB8668F0}" name="Outputs" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1126,7 +1164,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.6">
       <c r="A1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.6">
@@ -1146,10 +1184,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44549863-5D02-D84A-9B87-3FF43E548FC8}">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="74" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="74" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.84765625" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
@@ -1171,16 +1209,16 @@
         <v>14</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>109</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="62.4" x14ac:dyDescent="0.6">
@@ -1188,16 +1226,16 @@
         <v>7</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="46.8" x14ac:dyDescent="0.6">
@@ -1205,49 +1243,61 @@
         <v>9</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="171.6" x14ac:dyDescent="0.6">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="14" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="62.4" x14ac:dyDescent="0.6">
       <c r="A5" s="3" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>153</v>
+        <v>149</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>145</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>152</v>
+        <v>148</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="46.8" x14ac:dyDescent="0.6">
       <c r="A6" s="3" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>126</v>
+        <v>159</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="93.6" x14ac:dyDescent="0.6">
@@ -1255,16 +1305,16 @@
         <v>2</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="124.8" x14ac:dyDescent="0.6">
@@ -1272,19 +1322,19 @@
         <v>3</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>118</v>
+        <v>162</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="31.2" x14ac:dyDescent="0.6">
@@ -1292,15 +1342,15 @@
         <v>4</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="62.4" x14ac:dyDescent="0.6">
       <c r="A10" s="3" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="31.2" x14ac:dyDescent="0.6">
@@ -1308,7 +1358,7 @@
         <v>8</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="140.4" x14ac:dyDescent="0.6">
@@ -1316,27 +1366,27 @@
         <v>10</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="93.6" x14ac:dyDescent="0.6">
       <c r="A13" s="3" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="93.6" x14ac:dyDescent="0.6">
@@ -1344,22 +1394,25 @@
         <v>5</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>121</v>
+        <v>156</v>
       </c>
       <c r="C14" s="7"/>
       <c r="D14" s="8" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A15" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>107</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.6">
@@ -1370,10 +1423,10 @@
         <v>6</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.6">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.6">
       <c r="A17" s="3" t="s">
         <v>11</v>
       </c>
@@ -1381,7 +1434,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="18" spans="1:6" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A18" s="3" t="s">
         <v>13</v>
       </c>
@@ -1389,22 +1442,53 @@
         <v>106</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="19" spans="1:6" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A19" s="3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="46.8" x14ac:dyDescent="0.6">
+        <v>111</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="46.8" x14ac:dyDescent="0.6">
       <c r="B20" s="3" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="31.2" x14ac:dyDescent="0.6">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A21" s="3" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>159</v>
+        <v>155</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="171.6" x14ac:dyDescent="0.6">
+      <c r="A22" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.6">
+      <c r="A23" s="3" t="s">
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -1694,10 +1778,10 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A18" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C18" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -1721,10 +1805,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A1" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.6">

</xml_diff>

<commit_message>
Green are good to go; please review files in yellow.
</commit_message>
<xml_diff>
--- a/ptax_file_inventory.xlsx
+++ b/ptax_file_inventory.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleaw\Documents\PhD Fall 2021 - Spring 2022\Merriman RA\ptax\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micha\Data Analysis\ptax\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80B686D0-42AA-4E4E-9CA2-3490E9DFB11C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{556E0F6F-3A63-44F4-82D0-52F8E548D7B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" activeTab="1" xr2:uid="{8104F543-8E88-1346-A6A2-DCE31E170ED6}"/>
+    <workbookView xWindow="7780" yWindow="2080" windowWidth="28800" windowHeight="15370" activeTab="1" xr2:uid="{8104F543-8E88-1346-A6A2-DCE31E170ED6}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="3" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="177">
   <si>
     <t>File</t>
   </si>
@@ -60,9 +60,6 @@
     <t>merge_incentive_pins.R</t>
   </si>
   <si>
-    <t>Loop over PTAX datasets; call Cook County API</t>
-  </si>
-  <si>
     <t>0_joined_PIN_level_data_allyears.qmd</t>
   </si>
   <si>
@@ -360,9 +357,6 @@
     <t>ptax_pull_loop_* scripts</t>
   </si>
   <si>
-    <t>Pulls from ptaxsim.db and queries for freeze exemptions</t>
-  </si>
-  <si>
     <t>Typically build visualizations based on ptaxsim or merged PIN-level datasets</t>
   </si>
   <si>
@@ -393,34 +387,9 @@
     <t>Pulls all PINs that were EVER comm/ind from 2006-2023 that are within municipalities (i.e., no unincorporated areas of the county) for all years.</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>./Output/incentivePINs_allyears.csv,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> ./Necessary_Files/Assessor_-_Commercial_Valuation_Data_20240212.csv, ./Necessary_Files/Assessor_-_Commercial_Valuation_Data_20240301.csv, incentivePINs_accessDB_2.xlsx</t>
-    </r>
-  </si>
-  <si>
     <t>I don't think we need this file?</t>
   </si>
   <si>
-    <t>I think we want to pull the part of this document that makes the project data and put it in a separate script; jw did you do pre-2011 in a fit of nerd rage?</t>
-  </si>
-  <si>
     <t>Causal models using incentive class change as exogenous shock; does not aggregate to project level.</t>
   </si>
   <si>
@@ -460,9 +429,6 @@
     <t xml:space="preserve">Uses an archived parcel universe, ptaxsim, and the more current parcel universe to create keypins. </t>
   </si>
   <si>
-    <t>Might be old and redundant for a newer/better version in other files.</t>
-  </si>
-  <si>
     <t>methodology_reports/north_2022 folder, south_2023 folder,</t>
   </si>
   <si>
@@ -470,9 +436,6 @@
   </si>
   <si>
     <t xml:space="preserve">Combines the methodology worksheets found online and attempts to combine them. These worksheets become the "Commercial Valuation dataset" posted by the Assessor after significant data cleaning. This R script was an attempt to create them from scratch and see if it could be done better. Then got distracted with making keypins from the sales and appeals data identifiers. </t>
-  </si>
-  <si>
-    <t>Last ran and created files in May 2024, so the files are probably not used. It is a good example of how to read in a bunch of excel files though!</t>
   </si>
   <si>
     <t>Reads CCAO methodology spreadsheet files and combines them into 3 larget files for the Chicago, north, south, and triads for 2021, 2022, and 2023.</t>
@@ -607,6 +570,85 @@
   </si>
   <si>
     <t>Recreates all models included in the incentive report</t>
+  </si>
+  <si>
+    <t>Can this file be archived?</t>
+  </si>
+  <si>
+    <t>Loop over PTAX datasets for different levels of aggregation; call Cook County API</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Last ran and created files in May 2024, so the files are probably not used. It is a good example of how to read in a bunch of excel files though! </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Should we archive, then?</t>
+    </r>
+  </si>
+  <si>
+    <t>./Output/incentivePINs_allyears.csv, ./Necessary_Files/Assessor_-_Commercial_Valuation_Data_20240212.csv, ./Necessary_Files/Assessor_-_Commercial_Valuation_Data_20240301.csv, incentivePINs_accessDB_2.xlsx</t>
+  </si>
+  <si>
+    <t>Pulls from ptaxsim.db and queries for freeze exemptions to evaluate bills at different freeze levels.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Do we archive it in the meantime?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>I think we want to pull the part of this document that makes the project data and put it in a separate script; jw did you do pre-2011 in a fit of nerd rage?</t>
+    </r>
+  </si>
+  <si>
+    <t>Seems useful for case studies even if I have to change the year.</t>
+  </si>
+  <si>
+    <t>Creates simple statistics and visualizations about property tax revenues for local agencies.</t>
+  </si>
+  <si>
+    <t>This file is impressive and beautiful but I think it can be archived.</t>
+  </si>
+  <si>
+    <t>Doesn't seem to work with existing files? Might be old?</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Might be old and redundant for a newer/better version in other files. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Sounds like we should archive.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -636,13 +678,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="12"/>
       <color theme="1"/>
@@ -658,8 +693,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -669,18 +711,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -703,7 +733,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -715,34 +745,28 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1157,24 +1181,24 @@
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6484375" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="33.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.6">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.6">
-      <c r="A3" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1186,310 +1210,377 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44549863-5D02-D84A-9B87-3FF43E548FC8}">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="74" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" zoomScale="74" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.84765625" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="36.09765625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="40.69921875" style="3" customWidth="1"/>
+    <col min="1" max="1" width="36.08203125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="40.6640625" style="3" customWidth="1"/>
     <col min="3" max="3" width="31.25" style="3" customWidth="1"/>
-    <col min="4" max="4" width="28.84765625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="37.1484375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="26.34765625" style="3" customWidth="1"/>
-    <col min="7" max="16384" width="10.84765625" style="3"/>
+    <col min="4" max="4" width="28.83203125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="37.1640625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="26.33203125" style="3" customWidth="1"/>
+    <col min="7" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="62.4" x14ac:dyDescent="0.6">
-      <c r="A2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="E2" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="64" x14ac:dyDescent="0.4">
+      <c r="A2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="48" x14ac:dyDescent="0.4">
+      <c r="A3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+    </row>
+    <row r="4" spans="1:6" ht="176" x14ac:dyDescent="0.4">
+      <c r="A4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="64" x14ac:dyDescent="0.4">
+      <c r="A5" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="C5" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="46.8" x14ac:dyDescent="0.6">
-      <c r="A3" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="3" t="s">
+      <c r="F5" s="5" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="64" x14ac:dyDescent="0.4">
+      <c r="A6" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="171.6" x14ac:dyDescent="0.6">
-      <c r="A4" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="62.4" x14ac:dyDescent="0.6">
-      <c r="A5" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="B5" s="13" t="s">
-        <v>149</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="46.8" x14ac:dyDescent="0.6">
-      <c r="A6" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="93.6" x14ac:dyDescent="0.6">
+      <c r="C6" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="96" x14ac:dyDescent="0.4">
       <c r="A7" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="D7" s="3" t="s">
+      <c r="B7" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="144" x14ac:dyDescent="0.4">
+      <c r="A8" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="32" x14ac:dyDescent="0.4">
+      <c r="A9" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+    </row>
+    <row r="10" spans="1:6" ht="64" x14ac:dyDescent="0.4">
+      <c r="A10" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+    </row>
+    <row r="11" spans="1:6" ht="32" x14ac:dyDescent="0.4">
+      <c r="A11" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+    </row>
+    <row r="12" spans="1:6" ht="144" x14ac:dyDescent="0.4">
+      <c r="A12" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="E7" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="124.8" x14ac:dyDescent="0.6">
-      <c r="A8" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="A9" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="62.4" x14ac:dyDescent="0.6">
-      <c r="A10" s="3" t="s">
+      <c r="F12" s="4" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="96" x14ac:dyDescent="0.4">
+      <c r="A13" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="A11" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="140.4" x14ac:dyDescent="0.6">
-      <c r="A12" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="93.6" x14ac:dyDescent="0.6">
-      <c r="A13" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="93.6" x14ac:dyDescent="0.6">
+    </row>
+    <row r="14" spans="1:6" ht="96" x14ac:dyDescent="0.4">
       <c r="A14" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="C14" s="7"/>
-      <c r="D14" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="F14" s="3" t="s">
+      <c r="B14" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="32" x14ac:dyDescent="0.4">
+      <c r="A15" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C15" s="4"/>
+      <c r="D15" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+    </row>
+    <row r="16" spans="1:6" ht="32" x14ac:dyDescent="0.4">
+      <c r="A16" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+    </row>
+    <row r="17" spans="1:6" ht="48" x14ac:dyDescent="0.4">
+      <c r="A17" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" s="4"/>
+      <c r="D17" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+    </row>
+    <row r="18" spans="1:6" ht="48" x14ac:dyDescent="0.4">
+      <c r="A18" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+    </row>
+    <row r="19" spans="1:6" ht="32" x14ac:dyDescent="0.4">
+      <c r="A19" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+    </row>
+    <row r="20" spans="1:6" ht="48" x14ac:dyDescent="0.4">
+      <c r="A20" s="4"/>
+      <c r="B20" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+    </row>
+    <row r="21" spans="1:6" ht="32" x14ac:dyDescent="0.4">
+      <c r="A21" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="C21" s="4"/>
+      <c r="D21" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+    </row>
+    <row r="22" spans="1:6" ht="176" x14ac:dyDescent="0.4">
+      <c r="A22" s="5" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="A15" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.6">
-      <c r="A16" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.6">
-      <c r="A17" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="A18" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="A19" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="46.8" x14ac:dyDescent="0.6">
-      <c r="B20" s="3" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="A21" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="171.6" x14ac:dyDescent="0.6">
-      <c r="A22" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="32" x14ac:dyDescent="0.4">
+      <c r="A23" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="C22" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.6">
-      <c r="A23" s="3" t="s">
-        <v>170</v>
-      </c>
+      <c r="B23" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1508,280 +1599,280 @@
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6484375" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="57.1484375" customWidth="1"/>
-    <col min="3" max="3" width="50.1484375" customWidth="1"/>
-    <col min="4" max="4" width="32.1484375" customWidth="1"/>
+    <col min="1" max="1" width="57.1640625" customWidth="1"/>
+    <col min="3" max="3" width="50.1640625" customWidth="1"/>
+    <col min="4" max="4" width="32.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A2" s="1" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.6">
-      <c r="A2" s="1" t="s">
+      <c r="B2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>90</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A3" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>91</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.6">
-      <c r="A3" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>92</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.6">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>94</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A5" s="1" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.6">
-      <c r="A5" s="1" t="s">
-        <v>96</v>
-      </c>
       <c r="B5" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.6">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>97</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A7" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>91</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.6">
-      <c r="A7" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>92</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.6">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A9" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>91</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.6">
-      <c r="A9" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>92</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.6">
-      <c r="A10" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="1" t="s">
+      <c r="D11" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="D10" s="1" t="s">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A12" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.6">
-      <c r="A11" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.6">
-      <c r="A12" s="1" t="s">
-        <v>100</v>
-      </c>
       <c r="B12" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.6">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A13" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.6">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A14" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>102</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.6">
-      <c r="A15" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>103</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.6">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A16" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.6">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A17" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.6">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C18" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -1797,337 +1888,337 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6484375" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="46.6484375" customWidth="1"/>
+    <col min="1" max="1" width="46.6640625" customWidth="1"/>
     <col min="2" max="2" width="42.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.6">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A8" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A9" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A11" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A12" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A13" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A17" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A19" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A21" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A22" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A23" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A24" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A25" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A26" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A27" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A28" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A29" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A30" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A31" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A32" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A33" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A34" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A35" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A4" t="s">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A36" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A37" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A38" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A39" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A40" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A41" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A42" t="s">
+        <v>21</v>
+      </c>
+      <c r="B42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A43" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A44" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A45" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A6" t="s">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A46" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A47" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A48" t="s">
+        <v>31</v>
+      </c>
+      <c r="B48" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A49" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A50" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A51" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A52" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A53" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A54" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A55" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A56" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A57" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A58" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A59" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A8" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A9" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A10" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A11" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A12" t="s">
-        <v>59</v>
-      </c>
-      <c r="B12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A13" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A14" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A15" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A16" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.6">
-      <c r="A17" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.6">
-      <c r="A18" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.6">
-      <c r="A19" t="s">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A60" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A61" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.6">
-      <c r="A20" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.6">
-      <c r="A21" t="s">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A62" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.6">
-      <c r="A22" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.6">
-      <c r="A23" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.6">
-      <c r="A24" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.6">
-      <c r="A25" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.6">
-      <c r="A26" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.6">
-      <c r="A27" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.6">
-      <c r="A28" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.6">
-      <c r="A29" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.6">
-      <c r="A30" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.6">
-      <c r="A31" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.6">
-      <c r="A32" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A33" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A34" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A35" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A36" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A37" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A38" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A39" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A40" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A41" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A42" t="s">
-        <v>22</v>
-      </c>
-      <c r="B42" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A43" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A44" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A45" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A46" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A47" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.6">
-      <c r="A48" t="s">
-        <v>32</v>
-      </c>
-      <c r="B48" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.6">
-      <c r="A49" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.6">
-      <c r="A50" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.6">
-      <c r="A51" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.6">
-      <c r="A52" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.6">
-      <c r="A53" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.6">
-      <c r="A54" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.6">
-      <c r="A55" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.6">
-      <c r="A56" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.6">
-      <c r="A57" t="s">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A63" t="s">
         <v>77</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.6">
-      <c r="A58" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.6">
-      <c r="A59" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.6">
-      <c r="A60" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.6">
-      <c r="A61" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.6">
-      <c r="A62" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.6">
-      <c r="A63" t="s">
-        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -2146,7 +2237,7 @@
       <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6484375" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
moved archived files to separate archived tab
</commit_message>
<xml_diff>
--- a/ptax_file_inventory.xlsx
+++ b/ptax_file_inventory.xlsx
@@ -5,19 +5,20 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micha\Data Analysis\ptax\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleaw\Documents\PhD Fall 2021 - Spring 2022\Merriman RA\ptax\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{556E0F6F-3A63-44F4-82D0-52F8E548D7B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67F71B64-C9EF-4F72-A54C-2CCCA1224EE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7780" yWindow="2080" windowWidth="28800" windowHeight="15370" activeTab="1" xr2:uid="{8104F543-8E88-1346-A6A2-DCE31E170ED6}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="1" xr2:uid="{8104F543-8E88-1346-A6A2-DCE31E170ED6}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="3" r:id="rId1"/>
-    <sheet name="Sunnary (All)" sheetId="1" r:id="rId2"/>
-    <sheet name="Summary (Comm-Ind)" sheetId="5" r:id="rId3"/>
-    <sheet name="Output Sources" sheetId="4" r:id="rId4"/>
-    <sheet name="Changes to files" sheetId="6" r:id="rId5"/>
+    <sheet name="Summary (All)" sheetId="1" r:id="rId2"/>
+    <sheet name="Archived Files" sheetId="7" r:id="rId3"/>
+    <sheet name="Summary (Comm-Ind)" sheetId="5" r:id="rId4"/>
+    <sheet name="Output Sources" sheetId="4" r:id="rId5"/>
+    <sheet name="Changes to files" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="181">
   <si>
     <t>File</t>
   </si>
@@ -572,90 +573,56 @@
     <t>Recreates all models included in the incentive report</t>
   </si>
   <si>
-    <t>Can this file be archived?</t>
-  </si>
-  <si>
     <t>Loop over PTAX datasets for different levels of aggregation; call Cook County API</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Last ran and created files in May 2024, so the files are probably not used. It is a good example of how to read in a bunch of excel files though! </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Should we archive, then?</t>
-    </r>
-  </si>
-  <si>
     <t>./Output/incentivePINs_allyears.csv, ./Necessary_Files/Assessor_-_Commercial_Valuation_Data_20240212.csv, ./Necessary_Files/Assessor_-_Commercial_Valuation_Data_20240301.csv, incentivePINs_accessDB_2.xlsx</t>
   </si>
   <si>
     <t>Pulls from ptaxsim.db and queries for freeze exemptions to evaluate bills at different freeze levels.</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Do we archive it in the meantime?</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>I think we want to pull the part of this document that makes the project data and put it in a separate script; jw did you do pre-2011 in a fit of nerd rage?</t>
-    </r>
-  </si>
-  <si>
     <t>Seems useful for case studies even if I have to change the year.</t>
   </si>
   <si>
     <t>Creates simple statistics and visualizations about property tax revenues for local agencies.</t>
   </si>
   <si>
-    <t>This file is impressive and beautiful but I think it can be archived.</t>
-  </si>
-  <si>
     <t>Doesn't seem to work with existing files? Might be old?</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Might be old and redundant for a newer/better version in other files. </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Sounds like we should archive.</t>
-    </r>
+    <t>Archived?</t>
+  </si>
+  <si>
+    <t>Never Used</t>
+  </si>
+  <si>
+    <t>Last ran and created files in May 2024, so the files are probably not used. It is a good example of how to read in a bunch of excel files though!</t>
+  </si>
+  <si>
+    <t>Archived</t>
+  </si>
+  <si>
+    <t>Might be old and redundant for a newer/better version in other files.</t>
+  </si>
+  <si>
+    <t>I think we want to pull the part of this document that makes the project data and put it in a separate script</t>
+  </si>
+  <si>
+    <t>Move to website?</t>
+  </si>
+  <si>
+    <t>Move any parts to website?</t>
+  </si>
+  <si>
+    <t>Soon but not yet</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -700,8 +667,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -720,8 +695,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -729,11 +716,48 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -757,9 +781,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -769,11 +790,41 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="9">
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -827,18 +878,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{54438E1D-7E74-4957-AE8D-E2C5ABC9DAFB}" name="Table1" displayName="Table1" ref="A1:F23" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A1:F23" xr:uid="{54438E1D-7E74-4957-AE8D-E2C5ABC9DAFB}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F20">
-    <sortCondition ref="A1:A20"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{54438E1D-7E74-4957-AE8D-E2C5ABC9DAFB}" name="Table1" displayName="Table1" ref="A1:G17" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+  <autoFilter ref="A1:G17" xr:uid="{54438E1D-7E74-4957-AE8D-E2C5ABC9DAFB}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G17">
+    <sortCondition ref="G1:G17"/>
   </sortState>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{457F3B97-D78E-4D53-8E6B-FE920F1B7B60}" name="File" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{6B0D2B68-1EEC-48E8-BFB0-5D91728A5149}" name="Description" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{1BF32799-F320-46B3-A0F1-B24BE715E5B8}" name="Changes" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{FD59E246-87F8-4AEC-87F7-84E2B50D8F33}" name="Thoughts" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{7CFEA2D0-A2F5-4DC1-A26D-C81D47F75D97}" name="Inputs" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{F74E7965-C3AC-4B04-BEEC-DB75BB8668F0}" name="Outputs" dataDxfId="0"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{457F3B97-D78E-4D53-8E6B-FE920F1B7B60}" name="File" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{6B0D2B68-1EEC-48E8-BFB0-5D91728A5149}" name="Description" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{1BF32799-F320-46B3-A0F1-B24BE715E5B8}" name="Changes" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{FD59E246-87F8-4AEC-87F7-84E2B50D8F33}" name="Thoughts" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{7CFEA2D0-A2F5-4DC1-A26D-C81D47F75D97}" name="Inputs" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{F74E7965-C3AC-4B04-BEEC-DB75BB8668F0}" name="Outputs" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{386AB45E-518E-427F-9D16-4B28FAC39789}" name="Archived?" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1181,22 +1233,22 @@
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="10.6484375" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
   <cols>
     <col min="1" max="1" width="33.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.6">
       <c r="A1" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.6">
       <c r="A2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.6">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -1208,25 +1260,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44549863-5D02-D84A-9B87-3FF43E548FC8}">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="74" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
+      <selection pane="bottomLeft" activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="10.84765625" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
   <cols>
-    <col min="1" max="1" width="36.08203125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="40.6640625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="36.09765625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="40.6484375" style="3" customWidth="1"/>
     <col min="3" max="3" width="31.25" style="3" customWidth="1"/>
-    <col min="4" max="4" width="28.83203125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="37.1640625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="26.33203125" style="3" customWidth="1"/>
-    <col min="7" max="16384" width="10.83203125" style="3"/>
+    <col min="4" max="4" width="28.84765625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="37.1484375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="26.34765625" style="3" customWidth="1"/>
+    <col min="7" max="16384" width="10.84765625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1245,58 +1297,61 @@
       <c r="F1" s="2" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="64" x14ac:dyDescent="0.4">
+      <c r="G1" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="46.8" x14ac:dyDescent="0.6">
       <c r="A2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="3" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="A3" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="3" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="62.4" x14ac:dyDescent="0.6">
+      <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B4" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C4" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5" t="s">
+      <c r="D4" s="5"/>
+      <c r="E4" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F4" s="5" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="48" x14ac:dyDescent="0.4">
-      <c r="A3" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-    </row>
-    <row r="4" spans="1:6" ht="176" x14ac:dyDescent="0.4">
-      <c r="A4" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="64" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:7" ht="62.4" x14ac:dyDescent="0.6">
       <c r="A5" s="5" t="s">
         <v>141</v>
       </c>
@@ -1314,273 +1369,186 @@
         <v>152</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="64" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" ht="124.8" x14ac:dyDescent="0.6">
       <c r="A6" s="5" t="s">
-        <v>118</v>
+        <v>3</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="D6" s="5"/>
+        <v>114</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>124</v>
+      </c>
       <c r="E6" s="5" t="s">
-        <v>155</v>
+        <v>112</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="96" x14ac:dyDescent="0.4">
-      <c r="A7" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="144" x14ac:dyDescent="0.4">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="A7" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="1:7" ht="62.4" x14ac:dyDescent="0.6">
       <c r="A8" s="5" t="s">
-        <v>3</v>
+        <v>140</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="32" x14ac:dyDescent="0.4">
+        <v>147</v>
+      </c>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+    </row>
+    <row r="9" spans="1:7" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A9" s="5" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
     </row>
-    <row r="10" spans="1:6" ht="64" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:7" ht="140.4" x14ac:dyDescent="0.6">
       <c r="A10" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>147</v>
+        <v>9</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>135</v>
       </c>
       <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-    </row>
-    <row r="11" spans="1:6" ht="32" x14ac:dyDescent="0.4">
+      <c r="D10" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="93.6" x14ac:dyDescent="0.6">
       <c r="A11" s="5" t="s">
-        <v>7</v>
+        <v>144</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>117</v>
+        <v>145</v>
       </c>
       <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
+      <c r="D11" s="5" t="s">
+        <v>169</v>
+      </c>
       <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-    </row>
-    <row r="12" spans="1:6" ht="144" x14ac:dyDescent="0.4">
+      <c r="F11" s="5" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="93.6" x14ac:dyDescent="0.6">
       <c r="A12" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="96" x14ac:dyDescent="0.4">
+        <v>5</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A13" s="5" t="s">
-        <v>144</v>
+        <v>104</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5" t="s">
-        <v>172</v>
-      </c>
+        <v>166</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="D13" s="5"/>
       <c r="E13" s="5"/>
-      <c r="F13" s="5" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="96" x14ac:dyDescent="0.4">
-      <c r="A14" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>150</v>
-      </c>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12" t="s">
-        <v>115</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>169</v>
-      </c>
-      <c r="F14" s="11" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="32" x14ac:dyDescent="0.4">
-      <c r="A15" s="4" t="s">
-        <v>163</v>
-      </c>
+      <c r="F13" s="5"/>
+    </row>
+    <row r="14" spans="1:7" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="A14" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+    </row>
+    <row r="15" spans="1:7" ht="46.8" x14ac:dyDescent="0.6">
+      <c r="A15" s="4"/>
       <c r="B15" s="4" t="s">
-        <v>105</v>
+        <v>121</v>
       </c>
       <c r="C15" s="4"/>
-      <c r="D15" s="6" t="s">
-        <v>166</v>
-      </c>
+      <c r="D15" s="4"/>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" spans="1:6" ht="32" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:7" ht="171.6" x14ac:dyDescent="0.6">
       <c r="A16" s="5" t="s">
-        <v>104</v>
+        <v>157</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-    </row>
-    <row r="17" spans="1:6" ht="48" x14ac:dyDescent="0.4">
-      <c r="A17" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C17" s="4"/>
-      <c r="D17" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-    </row>
-    <row r="18" spans="1:6" ht="48" x14ac:dyDescent="0.4">
-      <c r="A18" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B18" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="A17" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-    </row>
-    <row r="19" spans="1:6" ht="32" x14ac:dyDescent="0.4">
-      <c r="A19" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-    </row>
-    <row r="20" spans="1:6" ht="48" x14ac:dyDescent="0.4">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-    </row>
-    <row r="21" spans="1:6" ht="32" x14ac:dyDescent="0.4">
-      <c r="A21" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="C21" s="4"/>
-      <c r="D21" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-    </row>
-    <row r="22" spans="1:6" ht="176" x14ac:dyDescent="0.4">
-      <c r="A22" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="32" x14ac:dyDescent="0.4">
-      <c r="A23" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1592,6 +1560,158 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E7902BE-B0B6-4A83-A207-DAA978852FE6}">
+  <dimension ref="A1:G7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="23.94921875" defaultRowHeight="224.7" customHeight="1" x14ac:dyDescent="0.6"/>
+  <sheetData>
+    <row r="1" spans="1:7" ht="26.4" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="224.7" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A2" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="224.7" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A3" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>153</v>
+      </c>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="G3" s="19" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="224.7" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A4" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16" t="s">
+        <v>176</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="F4" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="G4" s="17" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="224.7" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A5" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="C5" s="16"/>
+      <c r="D5" s="18" t="s">
+        <v>178</v>
+      </c>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="20" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="224.7" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A6" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="16"/>
+      <c r="D6" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="17" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="224.7" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A7" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>168</v>
+      </c>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="19" t="s">
+        <v>175</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB19EFBB-84B3-DC40-9462-4782F856E273}">
   <dimension ref="A1:E18"/>
   <sheetViews>
@@ -1599,14 +1719,14 @@
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="10.6484375" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
   <cols>
-    <col min="1" max="1" width="57.1640625" customWidth="1"/>
-    <col min="3" max="3" width="50.1640625" customWidth="1"/>
-    <col min="4" max="4" width="32.1640625" customWidth="1"/>
+    <col min="1" max="1" width="57.1484375" customWidth="1"/>
+    <col min="3" max="3" width="50.1484375" customWidth="1"/>
+    <col min="4" max="4" width="32.1484375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1623,7 +1743,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A2" s="1" t="s">
         <v>88</v>
       </c>
@@ -1638,7 +1758,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A3" s="1" t="s">
         <v>88</v>
       </c>
@@ -1653,7 +1773,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A4" s="1" t="s">
         <v>92</v>
       </c>
@@ -1668,7 +1788,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A5" s="1" t="s">
         <v>95</v>
       </c>
@@ -1683,7 +1803,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A6" s="1" t="s">
         <v>95</v>
       </c>
@@ -1698,7 +1818,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A7" s="1" t="s">
         <v>95</v>
       </c>
@@ -1713,7 +1833,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A8" s="1" t="s">
         <v>95</v>
       </c>
@@ -1728,7 +1848,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A9" s="1" t="s">
         <v>95</v>
       </c>
@@ -1743,7 +1863,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A10" s="1" t="s">
         <v>32</v>
       </c>
@@ -1760,7 +1880,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A11" s="1" t="s">
         <v>32</v>
       </c>
@@ -1777,7 +1897,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A12" s="1" t="s">
         <v>99</v>
       </c>
@@ -1792,7 +1912,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
@@ -1807,7 +1927,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A14" s="1" t="s">
         <v>17</v>
       </c>
@@ -1822,7 +1942,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A15" s="1" t="s">
         <v>17</v>
       </c>
@@ -1837,7 +1957,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A16" s="1" t="s">
         <v>17</v>
       </c>
@@ -1852,7 +1972,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
@@ -1867,7 +1987,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A18" t="s">
         <v>119</v>
       </c>
@@ -1880,7 +2000,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B518CB6C-64CD-4548-9867-37ED0B4CBCF0}">
   <dimension ref="A1:B63"/>
   <sheetViews>
@@ -1888,13 +2008,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="10.6484375" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
   <cols>
-    <col min="1" max="1" width="46.6640625" customWidth="1"/>
+    <col min="1" max="1" width="46.6484375" customWidth="1"/>
     <col min="2" max="2" width="42.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A1" t="s">
         <v>122</v>
       </c>
@@ -1902,57 +2022,57 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A3" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A4" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A5" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A6" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A8" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A9" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A10" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A11" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A12" t="s">
         <v>58</v>
       </c>
@@ -1960,152 +2080,152 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A13" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A14" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A15" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A16" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.6">
       <c r="A17" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.6">
       <c r="A18" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.6">
       <c r="A19" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.6">
       <c r="A20" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.6">
       <c r="A21" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.6">
       <c r="A22" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.6">
       <c r="A23" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.6">
       <c r="A24" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.6">
       <c r="A25" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.6">
       <c r="A26" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.6">
       <c r="A27" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.6">
       <c r="A28" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.6">
       <c r="A29" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.6">
       <c r="A30" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.6">
       <c r="A31" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.6">
       <c r="A32" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A33" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A34" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A35" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A36" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A37" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A38" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A39" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A40" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A41" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A42" t="s">
         <v>21</v>
       </c>
@@ -2113,32 +2233,32 @@
         <v>22</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A43" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A44" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A45" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A46" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A47" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A48" t="s">
         <v>31</v>
       </c>
@@ -2146,77 +2266,77 @@
         <v>32</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.6">
       <c r="A49" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.6">
       <c r="A50" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.6">
       <c r="A51" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.6">
       <c r="A52" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.6">
       <c r="A53" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.6">
       <c r="A54" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.6">
       <c r="A55" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.6">
       <c r="A56" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.6">
       <c r="A57" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.6">
       <c r="A58" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.6">
       <c r="A59" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.6">
       <c r="A60" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.6">
       <c r="A61" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.6">
       <c r="A62" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.6">
       <c r="A63" t="s">
         <v>77</v>
       </c>
@@ -2229,7 +2349,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C92558D-5ED6-EB4F-A2B4-CECE9826FD29}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -2237,7 +2357,7 @@
       <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="10.6484375" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
moved 2 files from archived tab to actively used tab (scripts for C&I project/pin cleaning)
</commit_message>
<xml_diff>
--- a/ptax_file_inventory.xlsx
+++ b/ptax_file_inventory.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleaw\Documents\PhD Fall 2021 - Spring 2022\Merriman RA\ptax\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67F71B64-C9EF-4F72-A54C-2CCCA1224EE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{489EBD72-4DC0-416E-BC68-D7D6BF870C43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="1" xr2:uid="{8104F543-8E88-1346-A6A2-DCE31E170ED6}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" firstSheet="1" activeTab="1" xr2:uid="{8104F543-8E88-1346-A6A2-DCE31E170ED6}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="3" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Archived Files" sheetId="7" r:id="rId3"/>
     <sheet name="Summary (Comm-Ind)" sheetId="5" r:id="rId4"/>
     <sheet name="Output Sources" sheetId="4" r:id="rId5"/>
-    <sheet name="Changes to files" sheetId="6" r:id="rId6"/>
+    <sheet name="Flowchart" sheetId="8" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="187">
   <si>
     <t>File</t>
   </si>
@@ -419,27 +419,6 @@
   </si>
   <si>
     <t>Produces list of tax codes and the municipality they are in.</t>
-  </si>
-  <si>
-    <t>all_keypins_2022.csv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">parceluniverse_keypins_20240725.xlsx, Assessor_-_Commercial_Valuation_Data_20240301.csv, amazonPINs.xlsx, helper_tc_muninames_2022.R, ptaxsim database, </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Uses an archived parcel universe, ptaxsim, and the more current parcel universe to create keypins. </t>
-  </si>
-  <si>
-    <t>methodology_reports/north_2022 folder, south_2023 folder,</t>
-  </si>
-  <si>
-    <t>Output/combined_methodologyworksheets_NORTH.csv, Output/combined_methodologyworksheets_SOUTH.csv, Output/combined_methodologyworksheets_CHICAGO.csv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Combines the methodology worksheets found online and attempts to combine them. These worksheets become the "Commercial Valuation dataset" posted by the Assessor after significant data cleaning. This R script was an attempt to create them from scratch and see if it could be done better. Then got distracted with making keypins from the sales and appeals data identifiers. </t>
-  </si>
-  <si>
-    <t>Reads CCAO methodology spreadsheet files and combines them into 3 larget files for the Chicago, north, south, and triads for 2021, 2022, and 2023.</t>
   </si>
   <si>
     <t xml:space="preserve">comm_ind_2011-2022 timeseries.csv, parceluniverse_keypins_20240724.xlsx, borappeals.csv, all_keypins.csv, </t>
@@ -507,9 +486,6 @@
     </r>
   </si>
   <si>
-    <t>mapping_com_ind_projects</t>
-  </si>
-  <si>
     <t>Identifies parcels that are owned by the same person. Maps a couple municipalities with the pins grouped by color</t>
   </si>
   <si>
@@ -597,15 +573,9 @@
     <t>Never Used</t>
   </si>
   <si>
-    <t>Last ran and created files in May 2024, so the files are probably not used. It is a good example of how to read in a bunch of excel files though!</t>
-  </si>
-  <si>
     <t>Archived</t>
   </si>
   <si>
-    <t>Might be old and redundant for a newer/better version in other files.</t>
-  </si>
-  <si>
     <t>I think we want to pull the part of this document that makes the project data and put it in a separate script</t>
   </si>
   <si>
@@ -616,6 +586,54 @@
   </si>
   <si>
     <t>Soon but not yet</t>
+  </si>
+  <si>
+    <t>Reads CCAO methodology spreadsheet files and combines them into 3 larger files for the Chicago, north, and South triads. Originally made for years 2021, 2022, and 2023. But has been updated with more recently updated City (2024) townships and North (2025) townships</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Combines the commercial valuation methodology worksheets found online and combines them. These worksheets become the "Commercial Valuation dataset" posted by the Assessor after significant data cleaning. This R script was an attempt to create them from scratch and unnest keypins and create common variables across tabs in the spreadsheet. </t>
+  </si>
+  <si>
+    <t>Output/combined_methodologyworksheets_north2025.csv, Output/combined_methodologyworksheets_chicago2024.csv Output/combined_methodologyworksheets_NORTH.csv, Output/combined_methodologyworksheets_SOUTH.csv, Output/combined_methodologyworksheets_CHICAGO.csv</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Cleans keypins and pins from commercial valuation worksheets.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">output/combined_methodologyworksheets_chicago2024.csv, ./output/combined_methodologyworksheets_north2025.csv, parceluniverse_keypins_20240725.xlsx, output/combined_methodologyworksheets_SOUTH,  Assessor_-_Commercial_Valuation_Data_20240301.csv, amazonPINs.xlsx, helper_tc_muninames_2022.R, ptaxsim database, </t>
+  </si>
+  <si>
+    <t>Output/keypins_from_methodwkshts.csv, all_keypins_2022.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inputs/methodologyreports/north_2025,  inputs/methodologyreports/chicago_2024, south_2023 folder, No longer used: methodology_reports/north_2022 folder &amp; Chicago 2021 folder, </t>
+  </si>
+  <si>
+    <t>Main Topic</t>
+  </si>
+  <si>
+    <t>Incentive PINs</t>
+  </si>
+  <si>
+    <t>C&amp;I Projects</t>
+  </si>
+  <si>
+    <t>Webste; All Topics</t>
+  </si>
+  <si>
+    <t>mapping_CI_projects</t>
+  </si>
+  <si>
+    <t>archive soon. Go through 1 more time</t>
+  </si>
+  <si>
+    <t>All Topics</t>
+  </si>
+  <si>
+    <t>Website; Incentive PINs</t>
   </si>
 </sst>
 </file>
@@ -708,7 +726,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -753,6 +771,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -790,38 +826,210 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="20">
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
+        <right style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </right>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -878,25 +1086,42 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{54438E1D-7E74-4957-AE8D-E2C5ABC9DAFB}" name="Table1" displayName="Table1" ref="A1:G17" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
-  <autoFilter ref="A1:G17" xr:uid="{54438E1D-7E74-4957-AE8D-E2C5ABC9DAFB}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G17">
-    <sortCondition ref="G1:G17"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{54438E1D-7E74-4957-AE8D-E2C5ABC9DAFB}" name="Table1" displayName="Table1" ref="A1:H19" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
+  <autoFilter ref="A1:H19" xr:uid="{54438E1D-7E74-4957-AE8D-E2C5ABC9DAFB}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G19">
+    <sortCondition ref="G1:G19"/>
   </sortState>
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{457F3B97-D78E-4D53-8E6B-FE920F1B7B60}" name="File" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{6B0D2B68-1EEC-48E8-BFB0-5D91728A5149}" name="Description" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{1BF32799-F320-46B3-A0F1-B24BE715E5B8}" name="Changes" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{FD59E246-87F8-4AEC-87F7-84E2B50D8F33}" name="Thoughts" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{7CFEA2D0-A2F5-4DC1-A26D-C81D47F75D97}" name="Inputs" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{F74E7965-C3AC-4B04-BEEC-DB75BB8668F0}" name="Outputs" dataDxfId="1"/>
-    <tableColumn id="8" xr3:uid="{386AB45E-518E-427F-9D16-4B28FAC39789}" name="Archived?" dataDxfId="0"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{457F3B97-D78E-4D53-8E6B-FE920F1B7B60}" name="File" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{6B0D2B68-1EEC-48E8-BFB0-5D91728A5149}" name="Description" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{1BF32799-F320-46B3-A0F1-B24BE715E5B8}" name="Changes" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{FD59E246-87F8-4AEC-87F7-84E2B50D8F33}" name="Thoughts" dataDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{7CFEA2D0-A2F5-4DC1-A26D-C81D47F75D97}" name="Inputs" dataDxfId="13"/>
+    <tableColumn id="6" xr3:uid="{F74E7965-C3AC-4B04-BEEC-DB75BB8668F0}" name="Outputs" dataDxfId="12"/>
+    <tableColumn id="8" xr3:uid="{386AB45E-518E-427F-9D16-4B28FAC39789}" name="Archived?" dataDxfId="11"/>
+    <tableColumn id="7" xr3:uid="{23F623BD-F124-48BF-9646-E331C898656D}" name="Main Topic" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{FB2AEC06-1224-485B-9AAA-A01041E10FC3}" name="Table3" displayName="Table3" ref="A1:G5" totalsRowShown="0" headerRowDxfId="1" dataDxfId="2" headerRowBorderDxfId="9" tableBorderDxfId="10" totalsRowBorderDxfId="8">
+  <autoFilter ref="A1:G5" xr:uid="{FB2AEC06-1224-485B-9AAA-A01041E10FC3}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{5FBFFDFC-42BB-4F49-AACA-66F486173BD3}" name="File" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{5A9AA585-9A10-4A92-A155-5FE46D7B753C}" name="Description" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{91458937-F768-4DB5-8850-EBBD37A9F871}" name="Changes" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{5F63D5E3-9562-4FD3-BB64-DDA5D360FD3E}" name="Thoughts"/>
+    <tableColumn id="5" xr3:uid="{5D46B301-7323-4003-B129-3793615ADCF9}" name="Inputs" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{DE371230-5697-4AE2-BBF9-5FE5A96324B9}" name="Outputs" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{5B3A69B1-2D0F-4F7E-9934-C5509177502D}" name="Archived?"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D84FAE05-F6C9-4A54-9026-E207569C7562}" name="Table2" displayName="Table2" ref="A1:B63" totalsRowShown="0">
   <autoFilter ref="A1:B63" xr:uid="{D84FAE05-F6C9-4A54-9026-E207569C7562}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B63">
@@ -1260,11 +1485,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44549863-5D02-D84A-9B87-3FF43E548FC8}">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.84765625" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
@@ -1278,7 +1503,7 @@
     <col min="7" max="16384" width="10.84765625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1298,10 +1523,13 @@
         <v>107</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="46.8" x14ac:dyDescent="0.6">
+        <v>164</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="46.8" x14ac:dyDescent="0.6">
       <c r="A2" s="5" t="s">
         <v>8</v>
       </c>
@@ -1313,242 +1541,315 @@
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
       <c r="G2" s="3" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="31.2" x14ac:dyDescent="0.6">
+        <v>165</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A3" s="4" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="6" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
       <c r="G3" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="62.4" x14ac:dyDescent="0.6">
-      <c r="A4" s="5" t="s">
+    <row r="4" spans="1:8" customFormat="1" ht="224.7" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A4" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>175</v>
+      </c>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13" t="s">
+        <v>176</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>177</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>174</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" customFormat="1" ht="224.7" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A5" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>172</v>
+      </c>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13" t="s">
+        <v>178</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>174</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="62.4" x14ac:dyDescent="0.6">
+      <c r="A6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="F4" s="5" t="s">
+      <c r="B6" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="62.4" x14ac:dyDescent="0.6">
+      <c r="A7" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="B7" s="7" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="62.4" x14ac:dyDescent="0.6">
-      <c r="A5" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="124.8" x14ac:dyDescent="0.6">
-      <c r="A6" s="5" t="s">
+      <c r="C7" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="124.8" x14ac:dyDescent="0.6">
+      <c r="A8" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B8" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C8" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D8" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E8" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="F6" s="5" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="A7" s="5" t="s">
+      <c r="F8" s="5" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="A9" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B9" s="5" t="s">
         <v>125</v>
-      </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-    </row>
-    <row r="8" spans="1:7" ht="62.4" x14ac:dyDescent="0.6">
-      <c r="A8" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-    </row>
-    <row r="9" spans="1:7" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="A9" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>117</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
     </row>
-    <row r="10" spans="1:7" ht="140.4" x14ac:dyDescent="0.6">
+    <row r="10" spans="1:8" ht="62.4" x14ac:dyDescent="0.6">
       <c r="A10" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="3" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="A11" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="H11" s="3" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="140.4" x14ac:dyDescent="0.6">
+      <c r="A12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="93.6" x14ac:dyDescent="0.6">
-      <c r="A11" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="93.6" x14ac:dyDescent="0.6">
-      <c r="A12" s="9" t="s">
+      <c r="B12" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="93.6" x14ac:dyDescent="0.6">
+      <c r="A13" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="93.6" x14ac:dyDescent="0.6">
+      <c r="A14" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B14" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="A15" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="H15" s="3" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="46.8" x14ac:dyDescent="0.6">
+      <c r="A16" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="H16" s="3" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="46.8" x14ac:dyDescent="0.6">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+    </row>
+    <row r="18" spans="1:6" ht="171.6" x14ac:dyDescent="0.6">
+      <c r="A18" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="B18" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>167</v>
-      </c>
-      <c r="F12" s="10" t="s">
+      <c r="C18" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="G12" s="3" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="A13" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-    </row>
-    <row r="14" spans="1:7" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="A14" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-    </row>
-    <row r="15" spans="1:7" ht="46.8" x14ac:dyDescent="0.6">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-    </row>
-    <row r="16" spans="1:7" ht="171.6" x14ac:dyDescent="0.6">
-      <c r="A16" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="D16" s="5" t="s">
+      <c r="D18" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="A19" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="B19" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="E16" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="A17" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1561,153 +1862,112 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E7902BE-B0B6-4A83-A207-DAA978852FE6}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView zoomScale="64" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.94921875" defaultRowHeight="224.7" customHeight="1" x14ac:dyDescent="0.6"/>
   <sheetData>
     <row r="1" spans="1:7" ht="26.4" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="18" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="G1" s="14" t="s">
-        <v>172</v>
+      <c r="G1" s="18" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="224.7" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A2" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>132</v>
-      </c>
-      <c r="C2" s="16" t="s">
-        <v>131</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>174</v>
-      </c>
-      <c r="E2" s="16" t="s">
-        <v>129</v>
-      </c>
-      <c r="F2" s="16" t="s">
-        <v>130</v>
-      </c>
-      <c r="G2" s="17" t="s">
-        <v>175</v>
+      <c r="A2" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="224.7" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A3" s="15" t="s">
-        <v>118</v>
-      </c>
-      <c r="B3" s="16" t="s">
-        <v>120</v>
-      </c>
-      <c r="C3" s="18" t="s">
-        <v>153</v>
-      </c>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16" t="s">
+      <c r="A3" s="13" t="s">
         <v>155</v>
       </c>
-      <c r="F3" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="G3" s="19" t="s">
-        <v>175</v>
+      <c r="B3" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="C3" s="13"/>
+      <c r="D3" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="224.7" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A4" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="16" t="s">
-        <v>128</v>
-      </c>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16" t="s">
-        <v>176</v>
-      </c>
-      <c r="E4" s="16" t="s">
-        <v>127</v>
-      </c>
-      <c r="F4" s="16" t="s">
-        <v>126</v>
-      </c>
+      <c r="A4" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="13"/>
+      <c r="D4" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
       <c r="G4" s="17" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="224.7" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A5" s="15" t="s">
-        <v>163</v>
-      </c>
-      <c r="B5" s="16" t="s">
-        <v>105</v>
-      </c>
-      <c r="C5" s="16"/>
-      <c r="D5" s="18" t="s">
-        <v>178</v>
-      </c>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
+      <c r="A5" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>160</v>
+      </c>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
       <c r="G5" s="20" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="224.7" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A6" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="18" t="s">
-        <v>179</v>
-      </c>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="17" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="224.7" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A7" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="16" t="s">
-        <v>168</v>
-      </c>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="19" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -2350,14 +2610,12 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C92558D-5ED6-EB4F-A2B4-CECE9826FD29}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E6F4558-CC52-43DB-BB73-BAF0433CB94D}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6484375" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
file tracker for project. not perfect but started
</commit_message>
<xml_diff>
--- a/ptax_file_inventory.xlsx
+++ b/ptax_file_inventory.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleaw\Documents\PhD Fall 2021 - Spring 2022\Merriman RA\ptax\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{489EBD72-4DC0-416E-BC68-D7D6BF870C43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{569829FF-B203-4A59-8BC5-6E7881E6A6FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" firstSheet="1" activeTab="1" xr2:uid="{8104F543-8E88-1346-A6A2-DCE31E170ED6}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{8104F543-8E88-1346-A6A2-DCE31E170ED6}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="3" r:id="rId1"/>
@@ -18,7 +18,6 @@
     <sheet name="Archived Files" sheetId="7" r:id="rId3"/>
     <sheet name="Summary (Comm-Ind)" sheetId="5" r:id="rId4"/>
     <sheet name="Output Sources" sheetId="4" r:id="rId5"/>
-    <sheet name="Flowchart" sheetId="8" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -100,12 +99,6 @@
     <t>QMD</t>
   </si>
   <si>
-    <t>Last updated: 6/3/2025</t>
-  </si>
-  <si>
-    <t>MVH</t>
-  </si>
-  <si>
     <t>Output File</t>
   </si>
   <si>
@@ -634,6 +627,12 @@
   </si>
   <si>
     <t>Website; Incentive PINs</t>
+  </si>
+  <si>
+    <t>Last updated: 11/9/2025 - AWM</t>
+  </si>
+  <si>
+    <t>Last updated: 6/3/2025 - MVH</t>
   </si>
 </sst>
 </file>
@@ -859,43 +858,6 @@
   </cellStyles>
   <dxfs count="20">
     <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="0"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -1009,13 +971,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color theme="4" tint="0.39997558519241921"/>
         </left>
@@ -1029,6 +984,50 @@
           <color theme="4" tint="0.39997558519241921"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1099,22 +1098,22 @@
     <tableColumn id="5" xr3:uid="{7CFEA2D0-A2F5-4DC1-A26D-C81D47F75D97}" name="Inputs" dataDxfId="13"/>
     <tableColumn id="6" xr3:uid="{F74E7965-C3AC-4B04-BEEC-DB75BB8668F0}" name="Outputs" dataDxfId="12"/>
     <tableColumn id="8" xr3:uid="{386AB45E-518E-427F-9D16-4B28FAC39789}" name="Archived?" dataDxfId="11"/>
-    <tableColumn id="7" xr3:uid="{23F623BD-F124-48BF-9646-E331C898656D}" name="Main Topic" dataDxfId="0"/>
+    <tableColumn id="7" xr3:uid="{23F623BD-F124-48BF-9646-E331C898656D}" name="Main Topic" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{FB2AEC06-1224-485B-9AAA-A01041E10FC3}" name="Table3" displayName="Table3" ref="A1:G5" totalsRowShown="0" headerRowDxfId="1" dataDxfId="2" headerRowBorderDxfId="9" tableBorderDxfId="10" totalsRowBorderDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{FB2AEC06-1224-485B-9AAA-A01041E10FC3}" name="Table3" displayName="Table3" ref="A1:G5" totalsRowShown="0" headerRowDxfId="9" dataDxfId="7" headerRowBorderDxfId="8" tableBorderDxfId="6" totalsRowBorderDxfId="5">
   <autoFilter ref="A1:G5" xr:uid="{FB2AEC06-1224-485B-9AAA-A01041E10FC3}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{5FBFFDFC-42BB-4F49-AACA-66F486173BD3}" name="File" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{5A9AA585-9A10-4A92-A155-5FE46D7B753C}" name="Description" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{91458937-F768-4DB5-8850-EBBD37A9F871}" name="Changes" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{5FBFFDFC-42BB-4F49-AACA-66F486173BD3}" name="File" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{5A9AA585-9A10-4A92-A155-5FE46D7B753C}" name="Description" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{91458937-F768-4DB5-8850-EBBD37A9F871}" name="Changes" dataDxfId="2"/>
     <tableColumn id="4" xr3:uid="{5F63D5E3-9562-4FD3-BB64-DDA5D360FD3E}" name="Thoughts"/>
-    <tableColumn id="5" xr3:uid="{5D46B301-7323-4003-B129-3793615ADCF9}" name="Inputs" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{DE371230-5697-4AE2-BBF9-5FE5A96324B9}" name="Outputs" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{5D46B301-7323-4003-B129-3793615ADCF9}" name="Inputs" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{DE371230-5697-4AE2-BBF9-5FE5A96324B9}" name="Outputs" dataDxfId="0"/>
     <tableColumn id="7" xr3:uid="{5B3A69B1-2D0F-4F7E-9934-C5509177502D}" name="Archived?"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1452,10 +1451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D03BF328-C577-0A45-9B47-87604B50A764}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6484375" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
@@ -1465,17 +1464,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.6">
       <c r="A1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.6">
-      <c r="A2" t="s">
-        <v>19</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.6">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>186</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.6">
+      <c r="A5" t="s">
+        <v>185</v>
       </c>
     </row>
   </sheetData>
@@ -1487,8 +1486,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44549863-5D02-D84A-9B87-3FF43E548FC8}">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="80" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
@@ -1511,22 +1510,22 @@
         <v>13</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="46.8" x14ac:dyDescent="0.6">
@@ -1534,37 +1533,37 @@
         <v>8</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
       <c r="G2" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A3" s="4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="6" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
       <c r="G3" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="4" spans="1:8" customFormat="1" ht="224.7" customHeight="1" x14ac:dyDescent="0.6">
@@ -1572,21 +1571,21 @@
         <v>2</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C4" s="13"/>
       <c r="D4" s="13"/>
       <c r="E4" s="13" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="5" spans="1:8" customFormat="1" ht="224.7" customHeight="1" x14ac:dyDescent="0.6">
@@ -1594,23 +1593,23 @@
         <v>1</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="G5" s="14" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="62.4" x14ac:dyDescent="0.6">
@@ -1618,38 +1617,38 @@
         <v>6</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="5" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="62.4" x14ac:dyDescent="0.6">
       <c r="A7" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B7" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="B7" s="7" t="s">
-        <v>136</v>
-      </c>
       <c r="C7" s="5" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="124.8" x14ac:dyDescent="0.6">
@@ -1657,19 +1656,19 @@
         <v>3</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="31.2" x14ac:dyDescent="0.6">
@@ -1677,7 +1676,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -1686,17 +1685,17 @@
     </row>
     <row r="10" spans="1:8" ht="62.4" x14ac:dyDescent="0.6">
       <c r="A10" s="5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
       <c r="G10" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="31.2" x14ac:dyDescent="0.6">
@@ -1704,14 +1703,14 @@
         <v>7</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
       <c r="H11" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="140.4" x14ac:dyDescent="0.6">
@@ -1719,39 +1718,39 @@
         <v>9</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="5" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="93.6" x14ac:dyDescent="0.6">
       <c r="A13" s="5" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="5" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E13" s="5"/>
       <c r="F13" s="5" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="93.6" x14ac:dyDescent="0.6">
@@ -1759,60 +1758,60 @@
         <v>5</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C14" s="11"/>
       <c r="D14" s="11" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A15" s="5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
       <c r="H15" s="3" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="46.8" x14ac:dyDescent="0.6">
       <c r="A16" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
       <c r="H16" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="46.8" x14ac:dyDescent="0.6">
       <c r="A17" s="4"/>
       <c r="B17" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
@@ -1821,30 +1820,30 @@
     </row>
     <row r="18" spans="1:6" ht="171.6" x14ac:dyDescent="0.6">
       <c r="A18" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="C18" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="D18" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="E18" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="F18" s="5" t="s">
         <v>151</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>152</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A19" s="5" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
@@ -1878,57 +1877,57 @@
         <v>13</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F1" s="18" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G1" s="18" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="224.7" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A2" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="B2" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="B2" s="13" t="s">
-        <v>120</v>
-      </c>
       <c r="C2" s="15" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D2" s="13"/>
       <c r="E2" s="13" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G2" s="16" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="224.7" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A3" s="13" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C3" s="13"/>
       <c r="D3" s="15" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E3" s="13"/>
       <c r="F3" s="13"/>
       <c r="G3" s="13" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="224.7" customHeight="1" x14ac:dyDescent="0.6">
@@ -1940,12 +1939,12 @@
       </c>
       <c r="C4" s="13"/>
       <c r="D4" s="15" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E4" s="13"/>
       <c r="F4" s="13"/>
       <c r="G4" s="17" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="224.7" customHeight="1" x14ac:dyDescent="0.6">
@@ -1953,14 +1952,14 @@
         <v>12</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C5" s="19"/>
       <c r="D5" s="19"/>
       <c r="E5" s="19"/>
       <c r="F5" s="19"/>
       <c r="G5" s="20" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -1991,185 +1990,185 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A2" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A3" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A4" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A5" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A6" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A7" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A8" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A9" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A10" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A11" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A12" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.6">
@@ -2180,11 +2179,11 @@
         <v>15</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.6">
@@ -2195,11 +2194,11 @@
         <v>15</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.6">
@@ -2210,11 +2209,11 @@
         <v>15</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.6">
@@ -2225,11 +2224,11 @@
         <v>15</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.6">
@@ -2240,19 +2239,19 @@
         <v>15</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.6">
       <c r="A18" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C18" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -2276,65 +2275,65 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A9" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A10" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A12" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B12" t="s">
         <v>14</v>
@@ -2342,263 +2341,263 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A13" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A14" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A15" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.6">
       <c r="A17" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.6">
       <c r="A18" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.6">
       <c r="A19" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.6">
       <c r="A20" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.6">
       <c r="A21" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.6">
       <c r="A22" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.6">
       <c r="A23" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.6">
       <c r="A24" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.6">
       <c r="A25" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.6">
       <c r="A26" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.6">
       <c r="A27" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.6">
       <c r="A28" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.6">
       <c r="A29" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.6">
       <c r="A30" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.6">
       <c r="A31" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.6">
       <c r="A32" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A33" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A34" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A35" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A36" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A37" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A38" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A39" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A40" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A41" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A42" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B42" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A43" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A44" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A45" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A46" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A47" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A48" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B48" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.6">
       <c r="A49" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.6">
       <c r="A50" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.6">
       <c r="A51" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.6">
       <c r="A52" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.6">
       <c r="A53" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.6">
       <c r="A54" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.6">
       <c r="A55" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.6">
       <c r="A56" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.6">
       <c r="A57" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.6">
       <c r="A58" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.6">
       <c r="A59" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.6">
       <c r="A60" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.6">
       <c r="A61" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.6">
       <c r="A62" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.6">
       <c r="A63" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -2607,16 +2606,4 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E6F4558-CC52-43DB-BB73-BAF0433CB94D}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>